<commit_message>
aggiunto codice, figure, edit minori dataset
</commit_message>
<xml_diff>
--- a/legislature_20210124.xlsx
+++ b/legislature_20210124.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roberto\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roberto\Desktop\rstudio_default\pol_fuoricontesto\legislature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3A171AE-2429-4219-927A-14490E3E3432}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{862DA143-ED90-4EAB-B081-1824C75AC9B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="13176" xr2:uid="{0AA036FD-B706-457C-9E38-E1111F2A78BC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="94">
   <si>
     <t>paese</t>
   </si>
@@ -313,6 +313,9 @@
   </si>
   <si>
     <t>https://pt.wikipedia.org/wiki/Assembleia_da_Rep%C3%BAblica</t>
+  </si>
+  <si>
+    <t>x+21</t>
   </si>
 </sst>
 </file>
@@ -395,8 +398,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{714C403F-AF67-41FE-B455-D5B93BEA0AAB}" name="Tabella1" displayName="Tabella1" ref="A1:I257" totalsRowShown="0">
-  <autoFilter ref="A1:I257" xr:uid="{57565825-99DD-4E25-888D-A8B563A6201A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{714C403F-AF67-41FE-B455-D5B93BEA0AAB}" name="Tabella1" displayName="Tabella1" ref="A1:I258" totalsRowShown="0">
+  <autoFilter ref="A1:I258" xr:uid="{57565825-99DD-4E25-888D-A8B563A6201A}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{618F1481-1CB5-4F15-A26B-ADBF71E98623}" name="paese"/>
     <tableColumn id="6" xr3:uid="{1527285D-6DBC-449D-97C5-59B773E384CB}" name="assemblea"/>
@@ -709,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB721021-4E39-4ED1-AF37-73AC7FFEE469}">
-  <dimension ref="A1:I257"/>
+  <dimension ref="A1:I258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="92" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A138" zoomScale="92" workbookViewId="0">
+      <selection activeCell="F160" sqref="F160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2957,7 +2960,7 @@
         <v>3</v>
       </c>
       <c r="D105" s="1">
-        <f t="shared" ref="D105:D168" si="2">E104</f>
+        <f t="shared" ref="D105:D169" si="2">E104</f>
         <v>29877</v>
       </c>
       <c r="E105" s="1">
@@ -4036,33 +4039,33 @@
         <v>36058</v>
       </c>
       <c r="E156" s="1">
+        <v>37514</v>
+      </c>
+      <c r="F156">
+        <v>4</v>
+      </c>
+      <c r="G156" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A157" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C157" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D157" s="5">
+        <f t="shared" si="2"/>
+        <v>37514</v>
+      </c>
+      <c r="E157" s="5">
         <v>38977</v>
       </c>
-      <c r="F156">
-        <v>4</v>
-      </c>
-      <c r="G156" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A157" t="s">
-        <v>45</v>
-      </c>
-      <c r="C157" t="s">
-        <v>63</v>
-      </c>
-      <c r="D157" s="1">
-        <f t="shared" si="2"/>
-        <v>38977</v>
-      </c>
-      <c r="E157" s="1">
-        <v>40440</v>
-      </c>
-      <c r="F157">
-        <v>4</v>
-      </c>
-      <c r="G157" t="s">
+      <c r="F157" s="4">
+        <v>4</v>
+      </c>
+      <c r="G157" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4070,15 +4073,14 @@
       <c r="A158" t="s">
         <v>45</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C158" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D158" s="1">
-        <f t="shared" si="2"/>
+      <c r="D158" s="5">
+        <v>38977</v>
+      </c>
+      <c r="E158" s="1">
         <v>40440</v>
-      </c>
-      <c r="E158" s="1">
-        <v>41896</v>
       </c>
       <c r="F158">
         <v>4</v>
@@ -4091,44 +4093,45 @@
       <c r="A159" t="s">
         <v>45</v>
       </c>
-      <c r="C159" t="s">
+      <c r="C159" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D159" s="1">
         <f t="shared" si="2"/>
+        <v>40440</v>
+      </c>
+      <c r="E159" s="1">
         <v>41896</v>
       </c>
-      <c r="E159" s="1">
-        <v>43352</v>
-      </c>
       <c r="F159">
         <v>4</v>
       </c>
       <c r="G159" t="s">
         <v>35</v>
-      </c>
-      <c r="H159" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>67</v>
-      </c>
-      <c r="C160">
-        <v>1</v>
+        <v>45</v>
+      </c>
+      <c r="C160" t="s">
+        <v>93</v>
       </c>
       <c r="D160" s="1">
-        <v>16983</v>
+        <f t="shared" si="2"/>
+        <v>41896</v>
       </c>
       <c r="E160" s="1">
-        <v>18195</v>
+        <v>43352</v>
       </c>
       <c r="F160">
         <v>4</v>
       </c>
       <c r="G160" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="H160" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.3">
@@ -4136,14 +4139,13 @@
         <v>67</v>
       </c>
       <c r="C161">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D161" s="1">
-        <f t="shared" si="2"/>
+        <v>16983</v>
+      </c>
+      <c r="E161" s="1">
         <v>18195</v>
-      </c>
-      <c r="E161" s="1">
-        <v>19538</v>
       </c>
       <c r="F161">
         <v>4</v>
@@ -4157,14 +4159,14 @@
         <v>67</v>
       </c>
       <c r="C162">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D162" s="1">
         <f t="shared" si="2"/>
+        <v>18195</v>
+      </c>
+      <c r="E162" s="1">
         <v>19538</v>
-      </c>
-      <c r="E162" s="1">
-        <v>20630</v>
       </c>
       <c r="F162">
         <v>4</v>
@@ -4178,14 +4180,14 @@
         <v>67</v>
       </c>
       <c r="C163">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D163" s="1">
         <f t="shared" si="2"/>
+        <v>19538</v>
+      </c>
+      <c r="E163" s="1">
         <v>20630</v>
-      </c>
-      <c r="E163" s="1">
-        <v>21729</v>
       </c>
       <c r="F163">
         <v>4</v>
@@ -4199,23 +4201,20 @@
         <v>67</v>
       </c>
       <c r="C164">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D164" s="1">
         <f t="shared" si="2"/>
+        <v>20630</v>
+      </c>
+      <c r="E164" s="1">
         <v>21729</v>
       </c>
-      <c r="E164" s="1">
-        <v>21849</v>
-      </c>
       <c r="F164">
         <v>4</v>
       </c>
       <c r="G164" t="s">
-        <v>35</v>
-      </c>
-      <c r="H164" t="s">
-        <v>69</v>
+        <v>36</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.3">
@@ -4223,20 +4222,23 @@
         <v>67</v>
       </c>
       <c r="C165">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D165" s="1">
         <f t="shared" si="2"/>
+        <v>21729</v>
+      </c>
+      <c r="E165" s="1">
         <v>21849</v>
       </c>
-      <c r="E165" s="1">
-        <v>23171</v>
-      </c>
       <c r="F165">
         <v>4</v>
       </c>
       <c r="G165" t="s">
         <v>35</v>
+      </c>
+      <c r="H165" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.3">
@@ -4244,14 +4246,14 @@
         <v>67</v>
       </c>
       <c r="C166">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D166" s="1">
         <f t="shared" si="2"/>
+        <v>21849</v>
+      </c>
+      <c r="E166" s="1">
         <v>23171</v>
-      </c>
-      <c r="E166" s="1">
-        <v>24634</v>
       </c>
       <c r="F166">
         <v>4</v>
@@ -4265,14 +4267,14 @@
         <v>67</v>
       </c>
       <c r="C167">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D167" s="1">
         <f t="shared" si="2"/>
+        <v>23171</v>
+      </c>
+      <c r="E167" s="1">
         <v>24634</v>
-      </c>
-      <c r="E167" s="1">
-        <v>26097</v>
       </c>
       <c r="F167">
         <v>4</v>
@@ -4286,14 +4288,14 @@
         <v>67</v>
       </c>
       <c r="C168">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D168" s="1">
         <f t="shared" si="2"/>
+        <v>24634</v>
+      </c>
+      <c r="E168" s="1">
         <v>26097</v>
-      </c>
-      <c r="E168" s="1">
-        <v>27210</v>
       </c>
       <c r="F168">
         <v>4</v>
@@ -4307,14 +4309,14 @@
         <v>67</v>
       </c>
       <c r="C169">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D169" s="1">
-        <f t="shared" ref="D169:D181" si="3">E168</f>
+        <f t="shared" si="2"/>
+        <v>26097</v>
+      </c>
+      <c r="E169" s="1">
         <v>27210</v>
-      </c>
-      <c r="E169" s="1">
-        <v>28666</v>
       </c>
       <c r="F169">
         <v>4</v>
@@ -4328,14 +4330,14 @@
         <v>67</v>
       </c>
       <c r="C170">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D170" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D170:D182" si="3">E169</f>
+        <v>27210</v>
+      </c>
+      <c r="E170" s="1">
         <v>28666</v>
-      </c>
-      <c r="E170" s="1">
-        <v>29192</v>
       </c>
       <c r="F170">
         <v>4</v>
@@ -4349,14 +4351,14 @@
         <v>67</v>
       </c>
       <c r="C171">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D171" s="1">
         <f t="shared" si="3"/>
+        <v>28666</v>
+      </c>
+      <c r="E171" s="1">
         <v>29192</v>
-      </c>
-      <c r="E171" s="1">
-        <v>30429</v>
       </c>
       <c r="F171">
         <v>4</v>
@@ -4370,14 +4372,14 @@
         <v>67</v>
       </c>
       <c r="C172">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D172" s="1">
         <f t="shared" si="3"/>
+        <v>29192</v>
+      </c>
+      <c r="E172" s="1">
         <v>30429</v>
-      </c>
-      <c r="E172" s="1">
-        <v>31892</v>
       </c>
       <c r="F172">
         <v>4</v>
@@ -4391,14 +4393,14 @@
         <v>67</v>
       </c>
       <c r="C173">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D173" s="1">
         <f t="shared" si="3"/>
+        <v>30429</v>
+      </c>
+      <c r="E173" s="1">
         <v>31892</v>
-      </c>
-      <c r="E173" s="1">
-        <v>33348</v>
       </c>
       <c r="F173">
         <v>4</v>
@@ -4412,14 +4414,14 @@
         <v>67</v>
       </c>
       <c r="C174">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D174" s="1">
         <f t="shared" si="3"/>
+        <v>31892</v>
+      </c>
+      <c r="E174" s="1">
         <v>33348</v>
-      </c>
-      <c r="E174" s="1">
-        <v>34797</v>
       </c>
       <c r="F174">
         <v>4</v>
@@ -4433,14 +4435,14 @@
         <v>67</v>
       </c>
       <c r="C175">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D175" s="1">
         <f t="shared" si="3"/>
+        <v>33348</v>
+      </c>
+      <c r="E175" s="1">
         <v>34797</v>
-      </c>
-      <c r="E175" s="1">
-        <v>36288</v>
       </c>
       <c r="F175">
         <v>4</v>
@@ -4454,14 +4456,14 @@
         <v>67</v>
       </c>
       <c r="C176">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D176" s="1">
         <f t="shared" si="3"/>
+        <v>34797</v>
+      </c>
+      <c r="E176" s="1">
         <v>36288</v>
-      </c>
-      <c r="E176" s="1">
-        <v>37751</v>
       </c>
       <c r="F176">
         <v>4</v>
@@ -4475,14 +4477,14 @@
         <v>67</v>
       </c>
       <c r="C177">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D177" s="1">
         <f t="shared" si="3"/>
+        <v>36288</v>
+      </c>
+      <c r="E177" s="1">
         <v>37751</v>
-      </c>
-      <c r="E177" s="1">
-        <v>39214</v>
       </c>
       <c r="F177">
         <v>4</v>
@@ -4496,14 +4498,14 @@
         <v>67</v>
       </c>
       <c r="C178">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D178" s="1">
         <f t="shared" si="3"/>
+        <v>37751</v>
+      </c>
+      <c r="E178" s="1">
         <v>39214</v>
-      </c>
-      <c r="E178" s="1">
-        <v>39928</v>
       </c>
       <c r="F178">
         <v>4</v>
@@ -4517,14 +4519,14 @@
         <v>67</v>
       </c>
       <c r="C179">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D179" s="1">
         <f t="shared" si="3"/>
+        <v>39214</v>
+      </c>
+      <c r="E179" s="1">
         <v>39928</v>
-      </c>
-      <c r="E179" s="1">
-        <v>41391</v>
       </c>
       <c r="F179">
         <v>4</v>
@@ -4538,14 +4540,14 @@
         <v>67</v>
       </c>
       <c r="C180">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D180" s="1">
         <f t="shared" si="3"/>
+        <v>39928</v>
+      </c>
+      <c r="E180" s="1">
         <v>41391</v>
-      </c>
-      <c r="E180" s="1">
-        <v>42672</v>
       </c>
       <c r="F180">
         <v>4</v>
@@ -4559,37 +4561,35 @@
         <v>67</v>
       </c>
       <c r="C181">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D181" s="1">
         <f t="shared" si="3"/>
+        <v>41391</v>
+      </c>
+      <c r="E181" s="1">
         <v>42672</v>
       </c>
-      <c r="E181" s="1">
-        <v>43036</v>
-      </c>
       <c r="F181">
         <v>4</v>
       </c>
       <c r="G181" t="s">
         <v>35</v>
-      </c>
-      <c r="H181" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C182">
-        <v>1</v>
-      </c>
-      <c r="D182" s="3">
-        <v>16939</v>
-      </c>
-      <c r="E182" s="3">
-        <v>17721</v>
+        <v>22</v>
+      </c>
+      <c r="D182" s="1">
+        <f t="shared" si="3"/>
+        <v>42672</v>
+      </c>
+      <c r="E182" s="1">
+        <v>43036</v>
       </c>
       <c r="F182">
         <v>4</v>
@@ -4598,7 +4598,7 @@
         <v>35</v>
       </c>
       <c r="H182" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.3">
@@ -4606,20 +4606,22 @@
         <v>70</v>
       </c>
       <c r="C183">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D183" s="3">
-        <f>E182</f>
+        <v>16939</v>
+      </c>
+      <c r="E183" s="3">
         <v>17721</v>
       </c>
-      <c r="E183" s="3">
-        <v>19170</v>
-      </c>
       <c r="F183">
         <v>4</v>
       </c>
       <c r="G183" t="s">
         <v>35</v>
+      </c>
+      <c r="H183" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.3">
@@ -4627,14 +4629,14 @@
         <v>70</v>
       </c>
       <c r="C184">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D184" s="3">
-        <f t="shared" ref="D184:D203" si="4">E183</f>
+        <f>E183</f>
+        <v>17721</v>
+      </c>
+      <c r="E184" s="3">
         <v>19170</v>
-      </c>
-      <c r="E184" s="3">
-        <v>20619</v>
       </c>
       <c r="F184">
         <v>4</v>
@@ -4648,23 +4650,20 @@
         <v>70</v>
       </c>
       <c r="C185">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D185" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="D185:D204" si="4">E184</f>
+        <v>19170</v>
+      </c>
+      <c r="E185" s="3">
         <v>20619</v>
       </c>
-      <c r="E185" s="3">
-        <v>21621</v>
-      </c>
       <c r="F185">
         <v>4</v>
       </c>
       <c r="G185" t="s">
         <v>35</v>
-      </c>
-      <c r="H185" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.3">
@@ -4672,21 +4671,23 @@
         <v>70</v>
       </c>
       <c r="C186">
-        <f>C185+1</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D186" s="3">
         <f t="shared" si="4"/>
+        <v>20619</v>
+      </c>
+      <c r="E186" s="3">
         <v>21621</v>
       </c>
-      <c r="E186" s="3">
-        <v>23146</v>
-      </c>
       <c r="F186">
         <v>4</v>
       </c>
       <c r="G186" t="s">
         <v>35</v>
+      </c>
+      <c r="H186" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.3">
@@ -4694,24 +4695,21 @@
         <v>70</v>
       </c>
       <c r="C187">
-        <f t="shared" ref="C187:C203" si="5">C186+1</f>
-        <v>6</v>
+        <f>C186+1</f>
+        <v>5</v>
       </c>
       <c r="D187" s="3">
         <f t="shared" si="4"/>
+        <v>21621</v>
+      </c>
+      <c r="E187" s="3">
         <v>23146</v>
       </c>
-      <c r="E187" s="3">
-        <v>24518</v>
-      </c>
       <c r="F187">
         <v>4</v>
       </c>
       <c r="G187" t="s">
         <v>35</v>
-      </c>
-      <c r="H187" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.3">
@@ -4719,16 +4717,16 @@
         <v>70</v>
       </c>
       <c r="C188">
-        <f t="shared" si="5"/>
-        <v>7</v>
+        <f t="shared" ref="C188:C204" si="5">C187+1</f>
+        <v>6</v>
       </c>
       <c r="D188" s="3">
         <f t="shared" si="4"/>
+        <v>23146</v>
+      </c>
+      <c r="E188" s="3">
         <v>24518</v>
       </c>
-      <c r="E188" s="3">
-        <v>26051</v>
-      </c>
       <c r="F188">
         <v>4</v>
       </c>
@@ -4736,7 +4734,7 @@
         <v>35</v>
       </c>
       <c r="H188" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.3">
@@ -4745,15 +4743,15 @@
       </c>
       <c r="C189">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D189" s="3">
         <f t="shared" si="4"/>
+        <v>24518</v>
+      </c>
+      <c r="E189" s="3">
         <v>26051</v>
       </c>
-      <c r="E189" s="3">
-        <v>26632</v>
-      </c>
       <c r="F189">
         <v>4</v>
       </c>
@@ -4761,7 +4759,7 @@
         <v>35</v>
       </c>
       <c r="H189" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.3">
@@ -4770,23 +4768,23 @@
       </c>
       <c r="C190">
         <f t="shared" si="5"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D190" s="3">
         <f t="shared" si="4"/>
+        <v>26051</v>
+      </c>
+      <c r="E190" s="3">
         <v>26632</v>
       </c>
-      <c r="E190" s="3">
-        <v>28270</v>
-      </c>
       <c r="F190">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G190" t="s">
         <v>35</v>
       </c>
       <c r="H190" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.3">
@@ -4795,20 +4793,23 @@
       </c>
       <c r="C191">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D191" s="3">
         <f t="shared" si="4"/>
+        <v>26632</v>
+      </c>
+      <c r="E191" s="3">
         <v>28270</v>
       </c>
-      <c r="E191" s="3">
-        <v>29732</v>
-      </c>
       <c r="F191">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G191" t="s">
         <v>35</v>
+      </c>
+      <c r="H191" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.3">
@@ -4817,23 +4818,20 @@
       </c>
       <c r="C192">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D192" s="3">
         <f t="shared" si="4"/>
+        <v>28270</v>
+      </c>
+      <c r="E192" s="3">
         <v>29732</v>
       </c>
-      <c r="E192" s="3">
-        <v>30202</v>
-      </c>
       <c r="F192">
         <v>4</v>
       </c>
       <c r="G192" t="s">
         <v>35</v>
-      </c>
-      <c r="H192" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.3">
@@ -4842,37 +4840,39 @@
       </c>
       <c r="C193">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D193" s="3">
         <f t="shared" si="4"/>
+        <v>29732</v>
+      </c>
+      <c r="E193" s="3">
         <v>30202</v>
       </c>
-      <c r="E193" s="3">
-        <v>31553</v>
-      </c>
       <c r="F193">
         <v>4</v>
       </c>
       <c r="G193" t="s">
         <v>35</v>
+      </c>
+      <c r="H193" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>70</v>
       </c>
-      <c r="B194" s="4"/>
       <c r="C194">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D194" s="3">
         <f t="shared" si="4"/>
+        <v>30202</v>
+      </c>
+      <c r="E194" s="3">
         <v>31553</v>
-      </c>
-      <c r="E194" s="3">
-        <v>32757</v>
       </c>
       <c r="F194">
         <v>4</v>
@@ -4885,25 +4885,23 @@
       <c r="A195" t="s">
         <v>70</v>
       </c>
+      <c r="B195" s="4"/>
       <c r="C195">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D195" s="3">
         <f t="shared" si="4"/>
+        <v>31553</v>
+      </c>
+      <c r="E195" s="3">
         <v>32757</v>
       </c>
-      <c r="E195" s="3">
-        <v>34457</v>
-      </c>
       <c r="F195">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G195" t="s">
         <v>35</v>
-      </c>
-      <c r="H195" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.3">
@@ -4912,20 +4910,23 @@
       </c>
       <c r="C196">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D196" s="3">
         <f t="shared" si="4"/>
+        <v>32757</v>
+      </c>
+      <c r="E196" s="3">
         <v>34457</v>
       </c>
-      <c r="E196" s="3">
-        <v>35921</v>
-      </c>
       <c r="F196">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G196" t="s">
         <v>35</v>
+      </c>
+      <c r="H196" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.3">
@@ -4934,23 +4935,20 @@
       </c>
       <c r="C197">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D197" s="3">
         <f t="shared" si="4"/>
+        <v>34457</v>
+      </c>
+      <c r="E197" s="3">
         <v>35921</v>
       </c>
-      <c r="E197" s="3">
-        <v>37391</v>
-      </c>
       <c r="F197">
         <v>4</v>
       </c>
       <c r="G197" t="s">
         <v>35</v>
-      </c>
-      <c r="H197" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.3">
@@ -4959,15 +4957,15 @@
       </c>
       <c r="C198">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D198" s="3">
         <f t="shared" si="4"/>
+        <v>35921</v>
+      </c>
+      <c r="E198" s="3">
         <v>37391</v>
       </c>
-      <c r="E198" s="3">
-        <v>37643</v>
-      </c>
       <c r="F198">
         <v>4</v>
       </c>
@@ -4975,7 +4973,7 @@
         <v>35</v>
       </c>
       <c r="H198" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.3">
@@ -4984,15 +4982,15 @@
       </c>
       <c r="C199">
         <f t="shared" si="5"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D199" s="3">
         <f t="shared" si="4"/>
+        <v>37391</v>
+      </c>
+      <c r="E199" s="3">
         <v>37643</v>
       </c>
-      <c r="E199" s="3">
-        <v>39043</v>
-      </c>
       <c r="F199">
         <v>4</v>
       </c>
@@ -5000,7 +4998,7 @@
         <v>35</v>
       </c>
       <c r="H199" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.3">
@@ -5009,23 +5007,23 @@
       </c>
       <c r="C200">
         <f t="shared" si="5"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D200" s="3">
         <f t="shared" si="4"/>
+        <v>37643</v>
+      </c>
+      <c r="E200" s="3">
         <v>39043</v>
       </c>
-      <c r="E200" s="3">
-        <v>40338</v>
-      </c>
       <c r="F200">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G200" t="s">
         <v>35</v>
       </c>
       <c r="H200" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.3">
@@ -5034,23 +5032,23 @@
       </c>
       <c r="C201">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D201" s="3">
         <f t="shared" si="4"/>
+        <v>39043</v>
+      </c>
+      <c r="E201" s="3">
         <v>40338</v>
       </c>
-      <c r="E201" s="3">
-        <v>41164</v>
-      </c>
       <c r="F201">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G201" t="s">
         <v>35</v>
       </c>
       <c r="H201" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.3">
@@ -5059,23 +5057,23 @@
       </c>
       <c r="C202">
         <f t="shared" si="5"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D202" s="3">
         <f t="shared" si="4"/>
+        <v>40338</v>
+      </c>
+      <c r="E202" s="3">
         <v>41164</v>
       </c>
-      <c r="E202" s="3">
-        <v>43034</v>
-      </c>
       <c r="F202">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G202" t="s">
         <v>35</v>
       </c>
       <c r="H202" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.3">
@@ -5084,47 +5082,49 @@
       </c>
       <c r="C203">
         <f t="shared" si="5"/>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D203" s="3">
         <f t="shared" si="4"/>
+        <v>41164</v>
+      </c>
+      <c r="E203" s="3">
         <v>43034</v>
       </c>
-      <c r="E203" s="3">
+      <c r="F203">
+        <v>5</v>
+      </c>
+      <c r="G203" t="s">
+        <v>35</v>
+      </c>
+      <c r="H203" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>70</v>
+      </c>
+      <c r="C204">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="D204" s="3">
+        <f t="shared" si="4"/>
+        <v>43034</v>
+      </c>
+      <c r="E204" s="3">
         <v>44272</v>
       </c>
-      <c r="F203">
-        <v>4</v>
-      </c>
-      <c r="G203" t="s">
-        <v>35</v>
-      </c>
-      <c r="H203" t="s">
+      <c r="F204">
+        <v>4</v>
+      </c>
+      <c r="G204" t="s">
+        <v>35</v>
+      </c>
+      <c r="H204" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A204" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B204" s="4"/>
-      <c r="C204" s="4">
-        <v>38</v>
-      </c>
-      <c r="D204" s="5">
-        <v>16664</v>
-      </c>
-      <c r="E204" s="5">
-        <v>18317</v>
-      </c>
-      <c r="F204" s="4">
-        <v>5</v>
-      </c>
-      <c r="G204" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H204" s="4"/>
-      <c r="I204" s="4"/>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A205" s="4" t="s">
@@ -5132,13 +5132,13 @@
       </c>
       <c r="B205" s="4"/>
       <c r="C205" s="4">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D205" s="5">
-        <v>18328</v>
+        <v>16664</v>
       </c>
       <c r="E205" s="5">
-        <v>18926</v>
+        <v>18317</v>
       </c>
       <c r="F205" s="4">
         <v>5</v>
@@ -5155,13 +5155,13 @@
       </c>
       <c r="B206" s="4"/>
       <c r="C206" s="4">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D206" s="5">
-        <v>18938</v>
+        <v>18328</v>
       </c>
       <c r="E206" s="5">
-        <v>20235</v>
+        <v>18926</v>
       </c>
       <c r="F206" s="4">
         <v>5</v>
@@ -5178,13 +5178,13 @@
       </c>
       <c r="B207" s="4"/>
       <c r="C207" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D207" s="5">
-        <v>20249</v>
+        <v>18938</v>
       </c>
       <c r="E207" s="5">
-        <v>21831</v>
+        <v>20235</v>
       </c>
       <c r="F207" s="4">
         <v>5</v>
@@ -5201,13 +5201,13 @@
       </c>
       <c r="B208" s="4"/>
       <c r="C208" s="4">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D208" s="5">
-        <v>21850</v>
+        <v>20249</v>
       </c>
       <c r="E208" s="5">
-        <v>23665</v>
+        <v>21831</v>
       </c>
       <c r="F208" s="4">
         <v>5</v>
@@ -5224,13 +5224,13 @@
       </c>
       <c r="B209" s="4"/>
       <c r="C209" s="4">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D209" s="5">
-        <v>23684</v>
+        <v>21850</v>
       </c>
       <c r="E209" s="5">
-        <v>24197</v>
+        <v>23665</v>
       </c>
       <c r="F209" s="4">
         <v>5</v>
@@ -5247,13 +5247,13 @@
       </c>
       <c r="B210" s="4"/>
       <c r="C210" s="4">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D210" s="5">
-        <v>24218</v>
+        <v>23684</v>
       </c>
       <c r="E210" s="5">
-        <v>25737</v>
+        <v>24197</v>
       </c>
       <c r="F210" s="4">
         <v>5</v>
@@ -5270,13 +5270,13 @@
       </c>
       <c r="B211" s="4"/>
       <c r="C211" s="4">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D211" s="5">
-        <v>25751</v>
+        <v>24218</v>
       </c>
       <c r="E211" s="5">
-        <v>27088</v>
+        <v>25737</v>
       </c>
       <c r="F211" s="4">
         <v>5</v>
@@ -5293,13 +5293,13 @@
       </c>
       <c r="B212" s="4"/>
       <c r="C212" s="4">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D212" s="5">
-        <v>27100</v>
+        <v>25751</v>
       </c>
       <c r="E212" s="5">
-        <v>27312</v>
+        <v>27088</v>
       </c>
       <c r="F212" s="4">
         <v>5</v>
@@ -5316,13 +5316,13 @@
       </c>
       <c r="B213" s="4"/>
       <c r="C213" s="4">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D213" s="5">
-        <v>27331</v>
+        <v>27100</v>
       </c>
       <c r="E213" s="5">
-        <v>28978</v>
+        <v>27312</v>
       </c>
       <c r="F213" s="4">
         <v>5</v>
@@ -5339,13 +5339,13 @@
       </c>
       <c r="B214" s="4"/>
       <c r="C214" s="4">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D214" s="5">
-        <v>28990</v>
+        <v>27331</v>
       </c>
       <c r="E214" s="5">
-        <v>30476</v>
+        <v>28978</v>
       </c>
       <c r="F214" s="4">
         <v>5</v>
@@ -5362,13 +5362,13 @@
       </c>
       <c r="B215" s="4"/>
       <c r="C215" s="4">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D215" s="5">
-        <v>30489</v>
+        <v>28990</v>
       </c>
       <c r="E215" s="5">
-        <v>31939</v>
+        <v>30476</v>
       </c>
       <c r="F215" s="4">
         <v>5</v>
@@ -5385,13 +5385,13 @@
       </c>
       <c r="B216" s="4"/>
       <c r="C216" s="4">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D216" s="5">
-        <v>31953</v>
+        <v>30489</v>
       </c>
       <c r="E216" s="5">
-        <v>33703</v>
+        <v>31939</v>
       </c>
       <c r="F216" s="4">
         <v>5</v>
@@ -5408,13 +5408,13 @@
       </c>
       <c r="B217" s="4"/>
       <c r="C217" s="4">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D217" s="5">
-        <v>33730</v>
+        <v>31953</v>
       </c>
       <c r="E217" s="5">
-        <v>35551</v>
+        <v>33703</v>
       </c>
       <c r="F217" s="4">
         <v>5</v>
@@ -5431,13 +5431,13 @@
       </c>
       <c r="B218" s="4"/>
       <c r="C218" s="4">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D218" s="5">
-        <v>35564</v>
+        <v>33730</v>
       </c>
       <c r="E218" s="5">
-        <v>37049</v>
+        <v>35551</v>
       </c>
       <c r="F218" s="4">
         <v>5</v>
@@ -5454,13 +5454,13 @@
       </c>
       <c r="B219" s="4"/>
       <c r="C219" s="4">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D219" s="5">
-        <v>37062</v>
+        <v>35564</v>
       </c>
       <c r="E219" s="5">
-        <v>38477</v>
+        <v>37049</v>
       </c>
       <c r="F219" s="4">
         <v>5</v>
@@ -5477,13 +5477,13 @@
       </c>
       <c r="B220" s="4"/>
       <c r="C220" s="4">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D220" s="5">
-        <v>38489</v>
+        <v>37062</v>
       </c>
       <c r="E220" s="5">
-        <v>40304</v>
+        <v>38477</v>
       </c>
       <c r="F220" s="4">
         <v>5</v>
@@ -5500,13 +5500,13 @@
       </c>
       <c r="B221" s="4"/>
       <c r="C221" s="4">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D221" s="5">
-        <v>40323</v>
+        <v>38489</v>
       </c>
       <c r="E221" s="5">
-        <v>42131</v>
+        <v>40304</v>
       </c>
       <c r="F221" s="4">
         <v>5</v>
@@ -5523,13 +5523,13 @@
       </c>
       <c r="B222" s="4"/>
       <c r="C222" s="4">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D222" s="5">
-        <v>42151</v>
+        <v>40323</v>
       </c>
       <c r="E222" s="5">
-        <v>42894</v>
+        <v>42131</v>
       </c>
       <c r="F222" s="4">
         <v>5</v>
@@ -5546,13 +5546,13 @@
       </c>
       <c r="B223" s="4"/>
       <c r="C223" s="4">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D223" s="5">
-        <v>42907</v>
+        <v>42151</v>
       </c>
       <c r="E223" s="5">
-        <v>43811</v>
+        <v>42894</v>
       </c>
       <c r="F223" s="4">
         <v>5</v>
@@ -5565,23 +5565,23 @@
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A224" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B224" s="4"/>
       <c r="C224" s="4">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="D224" s="5">
-        <v>16232</v>
+        <v>42907</v>
       </c>
       <c r="E224" s="5">
-        <v>17544</v>
+        <v>43811</v>
       </c>
       <c r="F224" s="4">
         <v>5</v>
       </c>
       <c r="G224" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H224" s="4"/>
       <c r="I224" s="4"/>
@@ -5592,13 +5592,13 @@
       </c>
       <c r="B225" s="4"/>
       <c r="C225" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D225" s="5">
-        <v>17581</v>
+        <v>16232</v>
       </c>
       <c r="E225" s="5">
-        <v>18755</v>
+        <v>17544</v>
       </c>
       <c r="F225" s="4">
         <v>5</v>
@@ -5615,13 +5615,13 @@
       </c>
       <c r="B226" s="4"/>
       <c r="C226" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D226" s="5">
-        <v>18792</v>
+        <v>17581</v>
       </c>
       <c r="E226" s="5">
-        <v>19838</v>
+        <v>18755</v>
       </c>
       <c r="F226" s="4">
         <v>5</v>
@@ -5629,6 +5629,8 @@
       <c r="G226" s="4" t="s">
         <v>88</v>
       </c>
+      <c r="H226" s="4"/>
+      <c r="I226" s="4"/>
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A227" s="4" t="s">
@@ -5636,13 +5638,13 @@
       </c>
       <c r="B227" s="4"/>
       <c r="C227" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D227" s="5">
-        <v>19877</v>
+        <v>18792</v>
       </c>
       <c r="E227" s="5">
-        <v>20863</v>
+        <v>19838</v>
       </c>
       <c r="F227" s="4">
         <v>5</v>
@@ -5657,13 +5659,13 @@
       </c>
       <c r="B228" s="4"/>
       <c r="C228" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D228" s="5">
-        <v>20899</v>
+        <v>19877</v>
       </c>
       <c r="E228" s="5">
-        <v>22539</v>
+        <v>20863</v>
       </c>
       <c r="F228" s="4">
         <v>5</v>
@@ -5678,13 +5680,13 @@
       </c>
       <c r="B229" s="4"/>
       <c r="C229" s="4">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D229" s="5">
-        <v>22565</v>
+        <v>20899</v>
       </c>
       <c r="E229" s="5">
-        <v>23819</v>
+        <v>22539</v>
       </c>
       <c r="F229" s="4">
         <v>5</v>
@@ -5699,13 +5701,13 @@
       </c>
       <c r="B230" s="4"/>
       <c r="C230" s="4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D230" s="5">
-        <v>23853</v>
+        <v>22565</v>
       </c>
       <c r="E230" s="5">
-        <v>25345</v>
+        <v>23819</v>
       </c>
       <c r="F230" s="4">
         <v>5</v>
@@ -5720,13 +5722,13 @@
       </c>
       <c r="B231" s="4"/>
       <c r="C231" s="4">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D231" s="5">
-        <v>25386</v>
+        <v>23853</v>
       </c>
       <c r="E231" s="5">
-        <v>26700</v>
+        <v>25345</v>
       </c>
       <c r="F231" s="4">
         <v>5</v>
@@ -5741,13 +5743,13 @@
       </c>
       <c r="B232" s="4"/>
       <c r="C232" s="4">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D232" s="5">
-        <v>26737</v>
+        <v>25386</v>
       </c>
       <c r="E232" s="5">
-        <v>28270</v>
+        <v>26700</v>
       </c>
       <c r="F232" s="4">
         <v>5</v>
@@ -5762,13 +5764,13 @@
       </c>
       <c r="B233" s="4"/>
       <c r="C233" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D233" s="5">
-        <v>28311</v>
+        <v>26737</v>
       </c>
       <c r="E233" s="5">
-        <v>29727</v>
+        <v>28270</v>
       </c>
       <c r="F233" s="4">
         <v>5</v>
@@ -5783,13 +5785,13 @@
       </c>
       <c r="B234" s="4"/>
       <c r="C234" s="4">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D234" s="5">
-        <v>29767</v>
+        <v>28311</v>
       </c>
       <c r="E234" s="5">
-        <v>29978</v>
+        <v>29727</v>
       </c>
       <c r="F234" s="4">
         <v>5</v>
@@ -5804,13 +5806,13 @@
       </c>
       <c r="B235" s="4"/>
       <c r="C235" s="4">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D235" s="5">
-        <v>30019</v>
+        <v>29767</v>
       </c>
       <c r="E235" s="5">
-        <v>30259</v>
+        <v>29978</v>
       </c>
       <c r="F235" s="4">
         <v>5</v>
@@ -5825,13 +5827,13 @@
       </c>
       <c r="B236" s="4"/>
       <c r="C236" s="4">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D236" s="5">
-        <v>30299</v>
+        <v>30019</v>
       </c>
       <c r="E236" s="5">
-        <v>31798</v>
+        <v>30259</v>
       </c>
       <c r="F236" s="4">
         <v>5</v>
@@ -5846,13 +5848,13 @@
       </c>
       <c r="B237" s="4"/>
       <c r="C237" s="4">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D237" s="5">
-        <v>31846</v>
+        <v>30299</v>
       </c>
       <c r="E237" s="5">
-        <v>32653</v>
+        <v>31798</v>
       </c>
       <c r="F237" s="4">
         <v>5</v>
@@ -5867,13 +5869,13 @@
       </c>
       <c r="B238" s="4"/>
       <c r="C238" s="4">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D238" s="5">
-        <v>32688</v>
+        <v>31846</v>
       </c>
       <c r="E238" s="5">
-        <v>33913</v>
+        <v>32653</v>
       </c>
       <c r="F238" s="4">
         <v>5</v>
@@ -5888,13 +5890,13 @@
       </c>
       <c r="B239" s="4"/>
       <c r="C239" s="4">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D239" s="5">
-        <v>33952</v>
+        <v>32688</v>
       </c>
       <c r="E239" s="5">
-        <v>35565</v>
+        <v>33913</v>
       </c>
       <c r="F239" s="4">
         <v>5</v>
@@ -5909,13 +5911,13 @@
       </c>
       <c r="B240" s="4"/>
       <c r="C240" s="4">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D240" s="5">
-        <v>35607</v>
+        <v>33952</v>
       </c>
       <c r="E240" s="5">
-        <v>37370</v>
+        <v>35565</v>
       </c>
       <c r="F240" s="4">
         <v>5</v>
@@ -5930,13 +5932,13 @@
       </c>
       <c r="B241" s="4"/>
       <c r="C241" s="4">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D241" s="5">
-        <v>37413</v>
+        <v>35607</v>
       </c>
       <c r="E241" s="5">
-        <v>39201</v>
+        <v>37370</v>
       </c>
       <c r="F241" s="4">
         <v>5</v>
@@ -5944,7 +5946,6 @@
       <c r="G241" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="H241" s="4"/>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A242" s="4" t="s">
@@ -5952,13 +5953,13 @@
       </c>
       <c r="B242" s="4"/>
       <c r="C242" s="4">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D242" s="5">
-        <v>39247</v>
+        <v>37413</v>
       </c>
       <c r="E242" s="5">
-        <v>40575</v>
+        <v>39201</v>
       </c>
       <c r="F242" s="4">
         <v>5</v>
@@ -5974,13 +5975,13 @@
       </c>
       <c r="B243" s="4"/>
       <c r="C243" s="4">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D243" s="5">
-        <v>40611</v>
+        <v>39247</v>
       </c>
       <c r="E243" s="5">
-        <v>42403</v>
+        <v>40575</v>
       </c>
       <c r="F243" s="4">
         <v>5</v>
@@ -5996,13 +5997,13 @@
       </c>
       <c r="B244" s="4"/>
       <c r="C244" s="4">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D244" s="5">
-        <v>42439</v>
+        <v>40611</v>
       </c>
       <c r="E244" s="5">
-        <v>43844</v>
+        <v>42403</v>
       </c>
       <c r="F244" s="4">
         <v>5</v>
@@ -6010,29 +6011,31 @@
       <c r="G244" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="H244" s="4" t="s">
-        <v>89</v>
-      </c>
+      <c r="H244" s="4"/>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A245" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B245" s="4"/>
       <c r="C245" s="4">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="D245" s="5">
-        <v>27875</v>
+        <v>42439</v>
       </c>
       <c r="E245" s="5">
-        <v>29191</v>
-      </c>
-      <c r="F245" s="4"/>
+        <v>43844</v>
+      </c>
+      <c r="F245" s="4">
+        <v>5</v>
+      </c>
       <c r="G245" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H245" s="4"/>
+        <v>88</v>
+      </c>
+      <c r="H245" s="4" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A246" s="4" t="s">
@@ -6040,15 +6043,17 @@
       </c>
       <c r="B246" s="4"/>
       <c r="C246" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D246" s="5">
-        <v>29499</v>
+        <v>27875</v>
       </c>
       <c r="E246" s="5">
-        <v>30431</v>
-      </c>
-      <c r="F246" s="4"/>
+        <v>29191</v>
+      </c>
+      <c r="F246" s="4">
+        <v>4</v>
+      </c>
       <c r="G246" s="4" t="s">
         <v>35</v>
       </c>
@@ -6060,15 +6065,17 @@
       </c>
       <c r="B247" s="4"/>
       <c r="C247" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D247" s="5">
+        <v>29499</v>
+      </c>
+      <c r="E247" s="5">
         <v>30431</v>
       </c>
-      <c r="E247" s="5">
-        <v>31326</v>
-      </c>
-      <c r="F247" s="4"/>
+      <c r="F247" s="4">
+        <v>4</v>
+      </c>
       <c r="G247" s="4" t="s">
         <v>35</v>
       </c>
@@ -6080,15 +6087,17 @@
       </c>
       <c r="B248" s="4"/>
       <c r="C248" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D248" s="5">
+        <v>30431</v>
+      </c>
+      <c r="E248" s="5">
         <v>31326</v>
       </c>
-      <c r="E248" s="5">
-        <v>31977</v>
-      </c>
-      <c r="F248" s="4"/>
+      <c r="F248" s="4">
+        <v>4</v>
+      </c>
       <c r="G248" s="4" t="s">
         <v>35</v>
       </c>
@@ -6100,15 +6109,17 @@
       </c>
       <c r="B249" s="4"/>
       <c r="C249" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D249" s="5">
+        <v>31326</v>
+      </c>
+      <c r="E249" s="5">
         <v>31977</v>
       </c>
-      <c r="E249" s="5">
-        <v>33517</v>
-      </c>
-      <c r="F249" s="4"/>
+      <c r="F249" s="4">
+        <v>4</v>
+      </c>
       <c r="G249" s="4" t="s">
         <v>35</v>
       </c>
@@ -6120,15 +6131,17 @@
       </c>
       <c r="B250" s="4"/>
       <c r="C250" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D250" s="5">
+        <v>31977</v>
+      </c>
+      <c r="E250" s="5">
         <v>33517</v>
       </c>
-      <c r="E250" s="5">
-        <v>34973</v>
-      </c>
-      <c r="F250" s="4"/>
+      <c r="F250" s="4">
+        <v>4</v>
+      </c>
       <c r="G250" s="4" t="s">
         <v>35</v>
       </c>
@@ -6140,15 +6153,17 @@
       </c>
       <c r="B251" s="4"/>
       <c r="C251" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D251" s="5">
+        <v>33517</v>
+      </c>
+      <c r="E251" s="5">
         <v>34973</v>
       </c>
-      <c r="E251" s="5">
-        <v>36443</v>
-      </c>
-      <c r="F251" s="4"/>
+      <c r="F251" s="4">
+        <v>4</v>
+      </c>
       <c r="G251" s="4" t="s">
         <v>35</v>
       </c>
@@ -6160,15 +6175,17 @@
       </c>
       <c r="B252" s="4"/>
       <c r="C252" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D252" s="5">
+        <v>34973</v>
+      </c>
+      <c r="E252" s="5">
         <v>36443</v>
       </c>
-      <c r="E252" s="5">
-        <v>37332</v>
-      </c>
-      <c r="F252" s="4"/>
+      <c r="F252" s="4">
+        <v>4</v>
+      </c>
       <c r="G252" s="4" t="s">
         <v>35</v>
       </c>
@@ -6180,15 +6197,17 @@
       </c>
       <c r="B253" s="4"/>
       <c r="C253" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D253" s="5">
+        <v>36443</v>
+      </c>
+      <c r="E253" s="5">
         <v>37332</v>
       </c>
-      <c r="E253" s="5">
-        <v>38403</v>
-      </c>
-      <c r="F253" s="4"/>
+      <c r="F253" s="4">
+        <v>4</v>
+      </c>
       <c r="G253" s="4" t="s">
         <v>35</v>
       </c>
@@ -6200,15 +6219,17 @@
       </c>
       <c r="B254" s="4"/>
       <c r="C254" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D254" s="5">
+        <v>37332</v>
+      </c>
+      <c r="E254" s="5">
         <v>38403</v>
       </c>
-      <c r="E254" s="5">
-        <v>40083</v>
-      </c>
-      <c r="F254" s="4"/>
+      <c r="F254" s="4">
+        <v>4</v>
+      </c>
       <c r="G254" s="4" t="s">
         <v>35</v>
       </c>
@@ -6220,15 +6241,17 @@
       </c>
       <c r="B255" s="4"/>
       <c r="C255" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D255" s="5">
+        <v>38403</v>
+      </c>
+      <c r="E255" s="5">
         <v>40083</v>
       </c>
-      <c r="E255" s="5">
-        <v>40699</v>
-      </c>
-      <c r="F255" s="4"/>
+      <c r="F255" s="4">
+        <v>4</v>
+      </c>
       <c r="G255" s="4" t="s">
         <v>35</v>
       </c>
@@ -6240,21 +6263,21 @@
       </c>
       <c r="B256" s="4"/>
       <c r="C256" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D256" s="5">
+        <v>40083</v>
+      </c>
+      <c r="E256" s="5">
         <v>40699</v>
       </c>
-      <c r="E256" s="5">
-        <v>42281</v>
-      </c>
-      <c r="F256" s="4"/>
+      <c r="F256" s="4">
+        <v>4</v>
+      </c>
       <c r="G256" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H256" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="H256" s="4"/>
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A257" s="4" t="s">
@@ -6262,19 +6285,45 @@
       </c>
       <c r="B257" s="4"/>
       <c r="C257" s="4">
+        <v>12</v>
+      </c>
+      <c r="D257" s="5">
+        <v>40699</v>
+      </c>
+      <c r="E257" s="5">
+        <v>42281</v>
+      </c>
+      <c r="F257" s="4">
+        <v>4</v>
+      </c>
+      <c r="G257" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H257" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A258" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B258" s="4"/>
+      <c r="C258" s="4">
         <v>13</v>
       </c>
-      <c r="D257" s="5">
+      <c r="D258" s="5">
         <v>42281</v>
       </c>
-      <c r="E257" s="5">
+      <c r="E258" s="5">
         <v>43744</v>
       </c>
-      <c r="F257" s="4"/>
-      <c r="G257" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H257" s="4" t="s">
+      <c r="F258" s="4">
+        <v>4</v>
+      </c>
+      <c r="G258" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H258" s="4" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>